<commit_message>
Adding BossPunching_Yellow.png 3 frames, 147x67 sheet size
</commit_message>
<xml_diff>
--- a/raw assets/Planning/KT-SpriteSheetGuide-BOSS.xlsx
+++ b/raw assets/Planning/KT-SpriteSheetGuide-BOSS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t xml:space="preserve">Kung Twu Sprite Sheet Breakdown - BOSS - YELLOW</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t xml:space="preserve">Punching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BossPunching_Yellow.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">147x67</t>
   </si>
   <si>
     <t xml:space="preserve">Kicking</t>
@@ -314,16 +320,16 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.61"/>
   </cols>
   <sheetData>
@@ -460,28 +466,32 @@
         <v>21</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>11</v>
@@ -501,7 +511,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -521,7 +531,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -541,7 +551,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -561,11 +571,11 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>11</v>
@@ -585,7 +595,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -605,7 +615,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>

</xml_diff>

<commit_message>
Added Boss Courching (1 frame) and Boss Crouch Punch (3 frames)
</commit_message>
<xml_diff>
--- a/raw assets/Planning/KT-SpriteSheetGuide-BOSS.xlsx
+++ b/raw assets/Planning/KT-SpriteSheetGuide-BOSS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t xml:space="preserve">Kung Twu Sprite Sheet Breakdown - BOSS - YELLOW</t>
   </si>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">Crouching</t>
   </si>
   <si>
+    <t xml:space="preserve">BossCrouching_Yellow.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">re-use frame 1 from sweeping?</t>
   </si>
   <si>
@@ -107,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">CrouchPunch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BossCrouchPunch_Yellow.png</t>
   </si>
   <si>
     <t xml:space="preserve">CrouchKick (Sweep)</t>
@@ -320,15 +326,15 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.61"/>
   </cols>
@@ -435,7 +441,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>4</v>
       </c>
@@ -443,19 +449,23 @@
         <v>19</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,11 +473,11 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>11</v>
@@ -476,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>13</v>
@@ -487,11 +497,11 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>11</v>
@@ -511,7 +521,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -531,7 +541,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -546,36 +556,40 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>11</v>
@@ -595,7 +609,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -615,7 +629,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>

</xml_diff>

<commit_message>
Updated Boss Kicking with new hair.  had to change frame size to 55x67 - 4 frames - spritesheet size 220x67
</commit_message>
<xml_diff>
--- a/raw assets/Planning/KT-SpriteSheetGuide-BOSS.xlsx
+++ b/raw assets/Planning/KT-SpriteSheetGuide-BOSS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t xml:space="preserve">Kung Twu Sprite Sheet Breakdown - BOSS - YELLOW</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t xml:space="preserve">BossKicking_Yellow.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55x67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220x67</t>
   </si>
   <si>
     <t xml:space="preserve">JumpPunch</t>
@@ -174,7 +180,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +191,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDAE3F3"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -229,7 +241,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -243,6 +255,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,7 +342,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -492,7 +508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>6</v>
       </c>
@@ -503,14 +519,14 @@
       <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>11</v>
+      <c r="E10" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>4</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>13</v>
@@ -521,7 +537,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -541,7 +557,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -561,11 +577,11 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>11</v>
@@ -585,11 +601,11 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>11</v>
@@ -609,7 +625,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -629,7 +645,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>

</xml_diff>